<commit_message>
Still lot more understanding required to pass the quiz and move ahead with Confusion matrix and other parameters
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
+++ b/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Course\Week-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21479292-FF6D-4EDF-8165-0EB6BAF4DA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="CM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,9 +108,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -262,7 +262,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -289,12 +289,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -580,11 +580,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,7 +600,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="49.5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -622,13 +622,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="6">
-        <v>429</v>
+        <v>96</v>
       </c>
       <c r="H3" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="49.5" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -642,13 +642,13 @@
         <v>6</v>
       </c>
       <c r="G4" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H4" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -662,82 +662,86 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11">
         <f>SUM(G3:H4)</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="15">
         <f>(G3+H4)/(D7)</f>
-        <v>0.98222222222222222</v>
+        <v>0.90551181102362199</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
+      <c r="K8" s="1">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="15">
         <f>1-D8</f>
-        <v>1.7777777777777781E-2</v>
+        <v>9.4488188976378007E-2</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <f>H4/(H4+G4)</f>
-        <v>0.8666666666666667</v>
+        <v>0.70370370370370372</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
+    <row r="11" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="C11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <f>H4/(H4+H3)</f>
-        <v>0.68421052631578949</v>
+        <v>0.82608695652173914</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="14" t="s">
+    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <f>H3/(G3+H3)</f>
-        <v>1.3793103448275862E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="14" t="s">
+    <row r="13" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <f>(2*H4)/(2*H4+G4+H3)</f>
-        <v>0.76470588235294112</v>
+        <v>0.76</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Test again failed online course - need deeper rereview
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
+++ b/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
@@ -111,9 +111,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +214,12 @@
       <color rgb="FF7030A0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -264,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -293,8 +299,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -581,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K13"/>
+  <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D9"/>
+      <selection activeCell="D8" sqref="D8:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -703,7 +710,7 @@
       <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="16">
         <f>H4/(H4+G4)</f>
         <v>0.70370370370370372</v>
       </c>
@@ -715,7 +722,7 @@
       <c r="C11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="16">
         <f>H4/(H4+H3)</f>
         <v>0.82608695652173914</v>
       </c>
@@ -727,7 +734,7 @@
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="16">
         <f>H3/(G3+H3)</f>
         <v>0.04</v>
       </c>
@@ -739,7 +746,7 @@
       <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="16">
         <f>(2*H4)/(2*H4+G4+H3)</f>
         <v>0.76</v>
       </c>
@@ -747,7 +754,34 @@
         <v>22</v>
       </c>
     </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="14">
+        <v>0.93463589743589703</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="14">
+        <v>0.90754658385093101</v>
+      </c>
+      <c r="H18" s="14">
+        <v>0.90767207564309005</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="1">
+        <f>G17-G18</f>
+        <v>2.7089313584966024E-2</v>
+      </c>
+      <c r="H19" s="1">
+        <f>H18-H17</f>
+        <v>-9.2327924356909952E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Evaluation metrics for ML models - study book also
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
+++ b/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Course\Week-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1429ED05-1516-4022-9C91-2F60F7F4F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -84,15 +85,9 @@
     <t>Recall</t>
   </si>
   <si>
-    <t xml:space="preserve"> (TP) / (TP + FN) - True positive rate / Sensitivity / Prob. Of detection</t>
-  </si>
-  <si>
     <t>Precision</t>
   </si>
   <si>
-    <t xml:space="preserve"> (TP) / (TP + FP) - Fraction of +ive predictions as correct</t>
-  </si>
-  <si>
     <t>Specificity</t>
   </si>
   <si>
@@ -103,15 +98,21 @@
   </si>
   <si>
     <t xml:space="preserve"> 2 x TP / (2 * TP + FN + FP) - Precision &amp; recall combined</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (TP) / (TP + FP) - True positive rate / Sensitivity / Prob. Of detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (TP) / (TP + FN) - Fraction of +ive predictions as correct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -268,7 +269,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -300,8 +301,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -587,11 +588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -607,7 +608,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -615,7 +616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -635,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -655,7 +656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -669,7 +670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
@@ -678,7 +679,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
@@ -689,12 +690,8 @@
       <c r="E8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="1">
-        <f>1/100</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
@@ -706,79 +703,60 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="16">
+        <f>H4/(H4+H3)</f>
+        <v>0.82608695652173914</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="C11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="16">
         <f>H4/(H4+G4)</f>
         <v>0.70370370370370372</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
+      <c r="E11" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="C12" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="D11" s="16">
-        <f>H4/(H4+H3)</f>
-        <v>0.82608695652173914</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="D12" s="16">
         <f>H3/(G3+H3)</f>
         <v>0.04</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="16">
         <f>(2*H4)/(2*H4+G4+H3)</f>
         <v>0.76</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G17" s="14">
-        <v>0.93463589743589703</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G18" s="14">
-        <v>0.90754658385093101</v>
-      </c>
-      <c r="H18" s="14">
-        <v>0.90767207564309005</v>
-      </c>
-    </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G19" s="1">
-        <f>G17-G18</f>
-        <v>2.7089313584966024E-2</v>
-      </c>
-      <c r="H19" s="1">
-        <f>H18-H17</f>
-        <v>-9.2327924356909952E-2</v>
-      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Almost near but still not there yet
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
+++ b/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Course\Week-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1429ED05-1516-4022-9C91-2F60F7F4F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="CM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Confusion Matrix</t>
   </si>
@@ -91,9 +90,6 @@
     <t>Specificity</t>
   </si>
   <si>
-    <t xml:space="preserve"> (TP) / (TP + FP) - False positive rate</t>
-  </si>
-  <si>
     <t>F1-Score</t>
   </si>
   <si>
@@ -104,17 +100,20 @@
   </si>
   <si>
     <t xml:space="preserve"> (TP) / (TP + FN) - Fraction of +ive predictions as correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (FP) / (TP + FP) - False positive rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +220,29 @@
       <color rgb="FF333333"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="40"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -269,9 +291,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,8 +323,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -588,11 +618,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -605,72 +635,106 @@
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="17"/>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5">
+        <v>96</v>
+      </c>
+      <c r="H3" s="8">
+        <v>4</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6">
-        <v>96</v>
-      </c>
-      <c r="H3" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>8</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="6">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="17"/>
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="L5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
@@ -679,7 +743,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
@@ -691,7 +755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
@@ -703,60 +767,63 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="16">
-        <f>H4/(H4+H3)</f>
-        <v>0.82608695652173914</v>
+        <f>(G3/(G3+G4))</f>
+        <v>0.92307692307692313</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="16">
-        <f>H4/(H4+G4)</f>
-        <v>0.70370370370370372</v>
+        <f>G3/(G3+H3)</f>
+        <v>0.96</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="C12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="16">
-        <f>H3/(G3+H3)</f>
-        <v>0.04</v>
+        <f>G4/(G3+G4)</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="C13" s="13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="16">
+        <f>(2*G3)/(2*G3+H3+G4)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="16">
-        <f>(2*H4)/(2*H4+G4+H3)</f>
-        <v>0.76</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Super happy that quiz almost done 76 percent now and almost there
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
+++ b/4_Applied ML with Python/Course/Week-3/Confusion Matrix.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Confusion Matrix</t>
   </si>
@@ -63,46 +63,25 @@
     <t>Pred Pos</t>
   </si>
   <si>
-    <t>User Input</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
     <t xml:space="preserve"> (TN + TP) / (Sum of all)</t>
   </si>
   <si>
-    <t>Error:</t>
-  </si>
-  <si>
     <t>Accuracy:</t>
   </si>
   <si>
-    <t xml:space="preserve"> (FN + FP) / (Sum of all)</t>
-  </si>
-  <si>
     <t>Recall</t>
   </si>
   <si>
     <t>Precision</t>
   </si>
   <si>
-    <t>Specificity</t>
-  </si>
-  <si>
-    <t>F1-Score</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 x TP / (2 * TP + FN + FP) - Precision &amp; recall combined</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (TP) / (TP + FP) - True positive rate / Sensitivity / Prob. Of detection</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (TP) / (TP + FN) - Fraction of +ive predictions as correct</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (FP) / (TP + FP) - False positive rate</t>
+    <t xml:space="preserve"> (TP) / (TP + FP) - Positive predictive value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (TP) / (TP + FN) - True positive rate / Sensitivity / Prob. Of detection</t>
   </si>
 </sst>
 </file>
@@ -113,7 +92,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,14 +115,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -157,30 +128,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="40"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="40"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="40"/>
-      <color rgb="FF0070C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="40"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF002060"/>
@@ -214,12 +161,6 @@
       <color rgb="FF7030A0"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -293,45 +234,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -619,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L18"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,197 +564,109 @@
     <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="17"/>
-      <c r="C2" s="18" t="s">
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="G2" s="2" t="s">
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="2:8" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="G5" s="5">
+        <f>SUM(C6:D7)</f>
+        <v>127</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="2:8" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="C6" s="12">
         <v>96</v>
       </c>
-      <c r="H3" s="8">
+      <c r="D6" s="12">
         <v>4</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="49.5" x14ac:dyDescent="0.2">
-      <c r="B4" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7">
+        <f>(C6+D7)/G5</f>
+        <v>0.90551181102362199</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="C7" s="12">
         <v>8</v>
       </c>
-      <c r="H4" s="6">
+      <c r="D7" s="12">
         <v>19</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="17"/>
-      <c r="C5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11">
-        <f>SUM(G3:H4)</f>
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C8" s="12" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="15">
-        <f>(G3+H4)/(D7)</f>
-        <v>0.90551181102362199</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C9" s="12" t="s">
+      <c r="G7" s="8">
+        <f>C6/(C6+C7)</f>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="15">
-        <f>1-D8</f>
-        <v>9.4488188976378007E-2</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+      <c r="G8" s="8">
+        <f>C6/(C6+D6)</f>
+        <v>0.96</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="16">
-        <f>(G3/(G3+G4))</f>
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="16">
-        <f>G3/(G3+H3)</f>
-        <v>0.96</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="16">
-        <f>G4/(G3+G4)</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="16">
-        <f>(2*G3)/(2*G3+H3+G4)</f>
-        <v>0.94117647058823528</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G17" s="14"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>